<commit_message>
created xml schema and xml file
</commit_message>
<xml_diff>
--- a/db/index_screen.xlsx
+++ b/db/index_screen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shangwen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shangwen\PhpstormProjects\lab_calculator\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,8 +24,16 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{78B79BF2-2C07-489B-B434-05158C68DC11}" name="index_schema" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Shangwen\PhpstormProjects\lab_calculator\db\index_schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="194">
   <si>
     <t>Tube</t>
   </si>
@@ -595,6 +603,21 @@
   </si>
   <si>
     <t>h12</t>
+  </si>
+  <si>
+    <t>tube</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>precipitant</t>
   </si>
 </sst>
 </file>
@@ -630,9 +653,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -650,6 +674,59 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
+<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
+  <Schema ID="Schema1">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="screen-condition">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="condition" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="tube" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="position" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="salt" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="buffer" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="precipitant" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Map ID="1" Name="screen-condition_Map" RootElement="screen-condition" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  </Map>
+</MapInfo>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{347A1EBB-C49E-4C0F-A59B-16874FF33F91}" name="Table1" displayName="Table1" ref="A1:E97" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:E97" xr:uid="{056BF7E9-7B29-4345-A542-A9CCCC08C254}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{48BE1C86-9F79-4E08-B9A3-3C5B63B21607}" uniqueName="tube" name="tube">
+      <xmlColumnPr mapId="1" xpath="/screen-condition/condition/tube" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{27BC55A0-72B1-4E20-8D95-96CF3B8648FA}" uniqueName="position" name="position">
+      <xmlColumnPr mapId="1" xpath="/screen-condition/condition/position" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{BD7BFD79-3CF1-4653-A2C2-2F2EAED3BA37}" uniqueName="salt" name="salt">
+      <xmlColumnPr mapId="1" xpath="/screen-condition/condition/salt" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{95D6ED67-A425-4009-B421-4163C96DD7D9}" uniqueName="buffer" name="buffer">
+      <xmlColumnPr mapId="1" xpath="/screen-condition/condition/buffer" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{31747430-64B1-4328-8E1F-3A0907E4335C}" uniqueName="precipitant" name="precipitant">
+      <xmlColumnPr mapId="1" xpath="/screen-condition/condition/precipitant" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C97995-B493-4DEC-8BB0-296DEFA5A1B6}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85:B96"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,1520 +1037,1581 @@
     <col min="1" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" customWidth="1"/>
+    <col min="5" max="5" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E34" t="s">
-        <v>37</v>
+      <c r="E34" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E35" t="s">
-        <v>38</v>
+      <c r="E35" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>36</v>
-      </c>
-      <c r="B36" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E36" t="s">
-        <v>39</v>
+      <c r="E36" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>39</v>
-      </c>
-      <c r="B39" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E39" t="s">
-        <v>42</v>
+      <c r="E39" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>42</v>
-      </c>
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>43</v>
-      </c>
-      <c r="B43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>45</v>
-      </c>
-      <c r="B45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>46</v>
-      </c>
-      <c r="B46" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E47" t="s">
-        <v>45</v>
+      <c r="E47" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>143</v>
-      </c>
-      <c r="C49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>50</v>
-      </c>
-      <c r="B50" t="s">
-        <v>144</v>
-      </c>
-      <c r="C50" t="s">
-        <v>97</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D51" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D52" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>53</v>
-      </c>
-      <c r="B53" t="s">
-        <v>147</v>
-      </c>
-      <c r="C53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D53" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>54</v>
-      </c>
-      <c r="B54" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" t="s">
-        <v>125</v>
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>55</v>
-      </c>
-      <c r="B55" t="s">
-        <v>149</v>
-      </c>
-      <c r="C55" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>56</v>
-      </c>
-      <c r="B56" t="s">
-        <v>150</v>
-      </c>
-      <c r="C56" t="s">
-        <v>100</v>
-      </c>
-      <c r="D56" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" t="s">
-        <v>126</v>
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>57</v>
-      </c>
-      <c r="B57" t="s">
-        <v>151</v>
-      </c>
-      <c r="C57" t="s">
-        <v>101</v>
-      </c>
-      <c r="D57" t="s">
-        <v>124</v>
-      </c>
-      <c r="E57" t="s">
-        <v>127</v>
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>58</v>
-      </c>
-      <c r="B58" t="s">
-        <v>152</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>128</v>
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>59</v>
-      </c>
-      <c r="B59" t="s">
-        <v>153</v>
-      </c>
-      <c r="C59" t="s">
-        <v>102</v>
-      </c>
-      <c r="D59" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" t="s">
-        <v>129</v>
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>60</v>
-      </c>
-      <c r="B60" t="s">
-        <v>154</v>
-      </c>
-      <c r="C60" t="s">
-        <v>103</v>
-      </c>
-      <c r="D60" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" t="s">
-        <v>130</v>
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>61</v>
-      </c>
-      <c r="B61" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61" t="s">
-        <v>104</v>
-      </c>
-      <c r="D61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" t="s">
-        <v>131</v>
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>62</v>
-      </c>
-      <c r="B62" t="s">
-        <v>156</v>
-      </c>
-      <c r="C62" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" t="s">
-        <v>132</v>
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>63</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="65" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>64</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" s="1" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>65</v>
-      </c>
-      <c r="B65" t="s">
-        <v>159</v>
-      </c>
-      <c r="C65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D65" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>66</v>
-      </c>
-      <c r="B66" t="s">
-        <v>160</v>
-      </c>
-      <c r="C66" t="s">
-        <v>108</v>
-      </c>
-      <c r="D66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E66" t="s">
-        <v>43</v>
+      <c r="E66" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>67</v>
-      </c>
-      <c r="B67" t="s">
-        <v>161</v>
-      </c>
-      <c r="C67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D67" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>68</v>
-      </c>
-      <c r="B68" t="s">
-        <v>162</v>
-      </c>
-      <c r="C68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D68" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>69</v>
-      </c>
-      <c r="B69" t="s">
-        <v>163</v>
-      </c>
-      <c r="C69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D69" t="s">
-        <v>14</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="D69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>70</v>
-      </c>
-      <c r="B70" t="s">
-        <v>164</v>
-      </c>
-      <c r="C70" t="s">
-        <v>109</v>
-      </c>
-      <c r="D70" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>71</v>
-      </c>
-      <c r="B71" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D71" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>72</v>
-      </c>
-      <c r="B72" t="s">
-        <v>166</v>
-      </c>
-      <c r="C72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D72" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="D72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>73</v>
-      </c>
-      <c r="B73" t="s">
-        <v>167</v>
-      </c>
-      <c r="C73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D73" t="s">
-        <v>14</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="D73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>74</v>
-      </c>
-      <c r="B74" t="s">
-        <v>168</v>
-      </c>
-      <c r="C74" t="s">
-        <v>110</v>
-      </c>
-      <c r="D74" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>75</v>
-      </c>
-      <c r="B75" t="s">
-        <v>169</v>
-      </c>
-      <c r="C75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="D75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>76</v>
-      </c>
-      <c r="B76" t="s">
-        <v>170</v>
-      </c>
-      <c r="C76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D76" t="s">
-        <v>13</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="D76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>77</v>
-      </c>
-      <c r="B77" t="s">
-        <v>171</v>
-      </c>
-      <c r="C77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D77" t="s">
-        <v>14</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="D77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>78</v>
-      </c>
-      <c r="B78" t="s">
-        <v>172</v>
-      </c>
-      <c r="C78" t="s">
-        <v>97</v>
-      </c>
-      <c r="D78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>79</v>
-      </c>
-      <c r="B79" t="s">
-        <v>173</v>
-      </c>
-      <c r="C79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D79" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="D79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>80</v>
-      </c>
-      <c r="B80" t="s">
-        <v>174</v>
-      </c>
-      <c r="C80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D80" t="s">
-        <v>13</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="D80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>81</v>
-      </c>
-      <c r="B81" t="s">
-        <v>175</v>
-      </c>
-      <c r="C81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D81" t="s">
-        <v>14</v>
-      </c>
-      <c r="E81" t="s">
+      <c r="D81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>82</v>
-      </c>
-      <c r="B82" t="s">
-        <v>176</v>
-      </c>
-      <c r="C82" t="s">
-        <v>111</v>
-      </c>
-      <c r="D82" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>83</v>
-      </c>
-      <c r="B83" t="s">
-        <v>177</v>
-      </c>
-      <c r="C83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D83" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="D83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>84</v>
-      </c>
-      <c r="B84" t="s">
-        <v>178</v>
-      </c>
-      <c r="C84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D84" t="s">
-        <v>13</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="D84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>85</v>
-      </c>
-      <c r="B85" t="s">
-        <v>66</v>
-      </c>
-      <c r="C85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D85" t="s">
-        <v>14</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="D85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>86</v>
-      </c>
-      <c r="B86" t="s">
-        <v>67</v>
-      </c>
-      <c r="C86" t="s">
-        <v>112</v>
-      </c>
-      <c r="D86" t="s">
-        <v>1</v>
-      </c>
-      <c r="E86" t="s">
-        <v>136</v>
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>87</v>
-      </c>
-      <c r="B87" t="s">
-        <v>179</v>
-      </c>
-      <c r="C87" t="s">
-        <v>113</v>
-      </c>
-      <c r="D87" t="s">
-        <v>1</v>
-      </c>
-      <c r="E87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>88</v>
-      </c>
-      <c r="B88" t="s">
-        <v>180</v>
-      </c>
-      <c r="C88" t="s">
-        <v>114</v>
-      </c>
-      <c r="D88" t="s">
-        <v>1</v>
-      </c>
-      <c r="E88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>89</v>
-      </c>
-      <c r="B89" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" t="s">
-        <v>115</v>
-      </c>
-      <c r="D89" t="s">
-        <v>1</v>
-      </c>
-      <c r="E89" t="s">
-        <v>137</v>
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>90</v>
-      </c>
-      <c r="B90" t="s">
-        <v>182</v>
-      </c>
-      <c r="C90" t="s">
-        <v>116</v>
-      </c>
-      <c r="D90" t="s">
-        <v>1</v>
-      </c>
-      <c r="E90" t="s">
-        <v>136</v>
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>91</v>
-      </c>
-      <c r="B91" t="s">
-        <v>183</v>
-      </c>
-      <c r="C91" t="s">
-        <v>117</v>
-      </c>
-      <c r="D91" t="s">
-        <v>1</v>
-      </c>
-      <c r="E91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>92</v>
-      </c>
-      <c r="B92" t="s">
-        <v>184</v>
-      </c>
-      <c r="C92" t="s">
-        <v>118</v>
-      </c>
-      <c r="D92" t="s">
-        <v>1</v>
-      </c>
-      <c r="E92" t="s">
-        <v>137</v>
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>93</v>
-      </c>
-      <c r="B93" t="s">
-        <v>185</v>
-      </c>
-      <c r="C93" t="s">
-        <v>119</v>
-      </c>
-      <c r="D93" t="s">
-        <v>1</v>
-      </c>
-      <c r="E93" t="s">
-        <v>136</v>
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>94</v>
-      </c>
-      <c r="B94" t="s">
-        <v>186</v>
-      </c>
-      <c r="C94" t="s">
-        <v>120</v>
-      </c>
-      <c r="D94" t="s">
-        <v>1</v>
-      </c>
-      <c r="E94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>95</v>
-      </c>
-      <c r="B95" t="s">
-        <v>187</v>
-      </c>
-      <c r="C95" t="s">
-        <v>121</v>
-      </c>
-      <c r="D95" t="s">
-        <v>1</v>
-      </c>
-      <c r="E95" t="s">
-        <v>138</v>
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
         <v>96</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D96" t="s">
-        <v>1</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="D97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>